<commit_message>
cleaned air quality data
</commit_message>
<xml_diff>
--- a/participant_meta_data/participant_meta_data.xlsx
+++ b/participant_meta_data/participant_meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcofking/Documents/GitHub/toilet_observational_study/participant_meta_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFD30E38-F5E4-E94B-A304-91C12C8EC097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A9B9E0-819A-EB42-8DFC-1EF99E5BB21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13020" yWindow="3880" windowWidth="43320" windowHeight="35360" xr2:uid="{DCC5170C-0A3E-7245-87B6-FB5476882216}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="51">
   <si>
     <t>participantID</t>
   </si>
@@ -131,13 +131,70 @@
   </si>
   <si>
     <t>experimentID</t>
+  </si>
+  <si>
+    <t>GT_012_W</t>
+  </si>
+  <si>
+    <t>GT_013_M</t>
+  </si>
+  <si>
+    <t>GT_014_W</t>
+  </si>
+  <si>
+    <t>GT_015_W</t>
+  </si>
+  <si>
+    <t>GT_016_W</t>
+  </si>
+  <si>
+    <t>GT_017_W</t>
+  </si>
+  <si>
+    <t>GT_018_W</t>
+  </si>
+  <si>
+    <t>GT_019_M</t>
+  </si>
+  <si>
+    <t>GT_020_M</t>
+  </si>
+  <si>
+    <t>GT_021_M</t>
+  </si>
+  <si>
+    <t>GT_022_M</t>
+  </si>
+  <si>
+    <t>GT_023_W</t>
+  </si>
+  <si>
+    <t>GT_024_M</t>
+  </si>
+  <si>
+    <t>GT_025_W</t>
+  </si>
+  <si>
+    <t>GT_026_W</t>
+  </si>
+  <si>
+    <t>GT_027_M</t>
+  </si>
+  <si>
+    <t>GT_028_M</t>
+  </si>
+  <si>
+    <t>GT_029_M</t>
+  </si>
+  <si>
+    <t>GT_030_M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +205,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,10 +237,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30620ADD-C2F2-9B4B-8374-4E1B05296CDB}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1664,6 +1730,946 @@
         <v>8</v>
       </c>
     </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="1">
+        <v>44771.442361111112</v>
+      </c>
+      <c r="D59" s="1">
+        <v>44771.444282407407</v>
+      </c>
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="1">
+        <v>44771.444444444445</v>
+      </c>
+      <c r="D60" s="1">
+        <v>44771.446006944447</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="1">
+        <v>44771.447222222225</v>
+      </c>
+      <c r="D61" s="1">
+        <v>44771.449317129627</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="1">
+        <v>44771.46597222222</v>
+      </c>
+      <c r="D62" s="1">
+        <v>44771.46707175926</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="1">
+        <v>44771.468055555553</v>
+      </c>
+      <c r="D63" s="1">
+        <v>44771.471990740742</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="1">
+        <v>44771.473611111112</v>
+      </c>
+      <c r="D64" s="1">
+        <v>44771.475138888891</v>
+      </c>
+      <c r="E64" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="1">
+        <v>44771.476388888892</v>
+      </c>
+      <c r="D65" s="1">
+        <v>44771.482314814813</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" s="1">
+        <v>44771.48333333333</v>
+      </c>
+      <c r="D66" s="1">
+        <v>44771.484780092593</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" s="1">
+        <v>44771.493055555555</v>
+      </c>
+      <c r="D67" s="1">
+        <v>44771.494328703702</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" s="1">
+        <v>44771.495138888888</v>
+      </c>
+      <c r="D68" s="1">
+        <v>44771.496863425928</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="1">
+        <v>44771.497916666667</v>
+      </c>
+      <c r="D69" s="1">
+        <v>44771.499837962961</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="1">
+        <v>44771.503472222219</v>
+      </c>
+      <c r="D70" s="1">
+        <v>44771.504340277781</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" s="1">
+        <v>44771.505555555559</v>
+      </c>
+      <c r="D71" s="1">
+        <v>44771.506990740738</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" s="1">
+        <v>44771.507638888892</v>
+      </c>
+      <c r="D72" s="1">
+        <v>44771.508692129632</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73" s="1">
+        <v>44771.57916666667</v>
+      </c>
+      <c r="D73" s="1">
+        <v>44771.580243055556</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>37</v>
+      </c>
+      <c r="C74" s="1">
+        <v>44771.581250000003</v>
+      </c>
+      <c r="D74" s="1">
+        <v>44771.541030092594</v>
+      </c>
+      <c r="E74" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" s="1">
+        <v>44771.583460648151</v>
+      </c>
+      <c r="D75" s="1">
+        <v>44771.585289351853</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" s="1">
+        <v>44771.586111111108</v>
+      </c>
+      <c r="D76" s="1">
+        <v>44771.586724537039</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" s="1">
+        <v>44771.587500000001</v>
+      </c>
+      <c r="D77" s="1">
+        <v>44771.590208333335</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78" s="1">
+        <v>44771.59034722222</v>
+      </c>
+      <c r="D78" s="1">
+        <v>44771.591666666667</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79" s="1">
+        <v>44771.593055555553</v>
+      </c>
+      <c r="D79" s="1">
+        <v>44771.593854166669</v>
+      </c>
+      <c r="E79" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C80" s="1">
+        <v>44771.594444444447</v>
+      </c>
+      <c r="D80" s="1">
+        <v>44771.595520833333</v>
+      </c>
+      <c r="E80" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81" s="1">
+        <v>44771.634722222225</v>
+      </c>
+      <c r="D81" s="1">
+        <v>44771.635949074072</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" s="1">
+        <v>44771.636805555558</v>
+      </c>
+      <c r="D82" s="1">
+        <v>44771.639907407407</v>
+      </c>
+      <c r="E82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C83" s="1">
+        <v>44771.64166666667</v>
+      </c>
+      <c r="D83" s="1">
+        <v>44771.642361111109</v>
+      </c>
+      <c r="E83" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84" s="1">
+        <v>44771.643055555556</v>
+      </c>
+      <c r="D84" s="1">
+        <v>44771.645312499997</v>
+      </c>
+      <c r="E84" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="1">
+        <v>44771.663888888892</v>
+      </c>
+      <c r="D85" s="1">
+        <v>44771.665277777778</v>
+      </c>
+      <c r="E85" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C86" s="1">
+        <v>44771.665972222225</v>
+      </c>
+      <c r="D86" s="1">
+        <v>44771.668923611112</v>
+      </c>
+      <c r="E86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" s="1">
+        <v>44771.68472222222</v>
+      </c>
+      <c r="D87" s="1">
+        <v>44771.685763888891</v>
+      </c>
+      <c r="E87" t="s">
+        <v>6</v>
+      </c>
+      <c r="F87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" s="1">
+        <v>44771.686805555553</v>
+      </c>
+      <c r="D88" s="1">
+        <v>44771.68854166667</v>
+      </c>
+      <c r="E88" t="s">
+        <v>6</v>
+      </c>
+      <c r="F88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C89" s="1">
+        <v>44771.69027777778</v>
+      </c>
+      <c r="D89" s="1">
+        <v>44771.691944444443</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+      <c r="F89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C90" s="1">
+        <v>44774.461111111108</v>
+      </c>
+      <c r="D90" s="1">
+        <v>44774.462337962963</v>
+      </c>
+      <c r="E90" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C91" s="1">
+        <v>44774.463194444441</v>
+      </c>
+      <c r="D91" s="1">
+        <v>44774.465578703705</v>
+      </c>
+      <c r="E91" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C92" s="1">
+        <v>44774.493055555555</v>
+      </c>
+      <c r="D92" s="1">
+        <v>44774.494467592594</v>
+      </c>
+      <c r="E92" t="s">
+        <v>6</v>
+      </c>
+      <c r="F92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C93" s="1">
+        <v>44774.495833333334</v>
+      </c>
+      <c r="D93" s="1">
+        <v>44774.498472222222</v>
+      </c>
+      <c r="E93" t="s">
+        <v>6</v>
+      </c>
+      <c r="F93" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C94" s="1">
+        <v>44774.499305555553</v>
+      </c>
+      <c r="D94" s="1">
+        <v>44774.501840277779</v>
+      </c>
+      <c r="E94" t="s">
+        <v>6</v>
+      </c>
+      <c r="F94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C95" s="1">
+        <v>44774.50277777778</v>
+      </c>
+      <c r="D95" s="1">
+        <v>44774.504293981481</v>
+      </c>
+      <c r="E95" t="s">
+        <v>6</v>
+      </c>
+      <c r="F95" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C96" s="1">
+        <v>44774.504861111112</v>
+      </c>
+      <c r="D96" s="1">
+        <v>44774.507141203707</v>
+      </c>
+      <c r="E96" t="s">
+        <v>6</v>
+      </c>
+      <c r="F96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" s="1">
+        <v>44774.508333333331</v>
+      </c>
+      <c r="D97" s="1">
+        <v>44774.51059027778</v>
+      </c>
+      <c r="E97" t="s">
+        <v>6</v>
+      </c>
+      <c r="F97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C98" s="1">
+        <v>44774.529861111114</v>
+      </c>
+      <c r="D98" s="1">
+        <v>44774.530729166669</v>
+      </c>
+      <c r="E98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99" s="1">
+        <v>44774.53125</v>
+      </c>
+      <c r="D99" s="1">
+        <v>44774.532650462963</v>
+      </c>
+      <c r="E99" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C100" s="1">
+        <v>44774.585416666669</v>
+      </c>
+      <c r="D100" s="1">
+        <v>44774.586840277778</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C101" s="1">
+        <v>44774.587500000001</v>
+      </c>
+      <c r="D101" s="1">
+        <v>44774.591157407405</v>
+      </c>
+      <c r="E101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C102" s="1">
+        <v>44774.630555555559</v>
+      </c>
+      <c r="D102" s="1">
+        <v>44774.631944444445</v>
+      </c>
+      <c r="E102" t="s">
+        <v>9</v>
+      </c>
+      <c r="F102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C103" s="1">
+        <v>44774.632638888892</v>
+      </c>
+      <c r="D103" s="1">
+        <v>44774.635787037034</v>
+      </c>
+      <c r="E103" t="s">
+        <v>9</v>
+      </c>
+      <c r="F103" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C104" s="1">
+        <v>44774.647916666669</v>
+      </c>
+      <c r="D104" s="1">
+        <v>44774.6487037037</v>
+      </c>
+      <c r="E104" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C105" s="1">
+        <v>44774.649305555555</v>
+      </c>
+      <c r="D105" s="1">
+        <v>44774.65079861111</v>
+      </c>
+      <c r="E105" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>